<commit_message>
Fixed alignment and template
</commit_message>
<xml_diff>
--- a/src/apps/researches/templates/daily_export.xlsx
+++ b/src/apps/researches/templates/daily_export.xlsx
@@ -341,6 +341,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -360,7 +361,7 @@
     <row r="1">
       <c r="A1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" ht="36.0" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -395,6 +396,9 @@
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A1:J1"/>
   </mergeCells>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>